<commit_message>
Added on 20, 2017
</commit_message>
<xml_diff>
--- a/Resources/ZCustomaization.xlsx
+++ b/Resources/ZCustomaization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>User Name</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>Schedule Number Counter</t>
+  </si>
+  <si>
+    <t>Data Recorder Index</t>
   </si>
 </sst>
 </file>
@@ -406,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +478,7 @@
       </c>
       <c r="G6" s="2">
         <f ca="1">TODAY()</f>
-        <v>42997</v>
+        <v>42998</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="2"/>
@@ -484,7 +490,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3012633024</v>
+        <v>3013685163</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -505,12 +511,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
3-remove login credentials from data script
</commit_message>
<xml_diff>
--- a/Resources/ZCustomaization.xlsx
+++ b/Resources/ZCustomaization.xlsx
@@ -1,34 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="true" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
-  <si>
-    <t>User Name</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>SERVICE$08</t>
-  </si>
-  <si>
-    <t>AgsautoT04</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>CO#</t>
   </si>
@@ -63,12 +51,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mmddyyyy"/>
     <numFmt numFmtId="165" formatCode="0_);\(0\)"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,17 +87,50 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="true" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -399,58 +420,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A5:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="15.28515625" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="12.5703125" bestFit="true" customWidth="true"/>
-    <col min="8" max="8" width="15.28515625" style="2" bestFit="true" customWidth="true"/>
-    <col min="9" max="9" width="9.7109375" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3013684357</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="4"/>
@@ -458,164 +463,164 @@
       <c r="H6" s="3"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3013695991</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>3013649705</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>3013410769</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>3013600797</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>3013650984</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>3013650989</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>3013667080</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>3013676007</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>3013696116</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>3013696125</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>3013696128</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>3013696132</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>3013696136</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>3013696159</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>3013410769</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>3013490006</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>3013527955</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>3013628150</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>3013629116</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>3013629139</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -625,29 +630,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -659,12 +664,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
3-change order quantity to 1
reduces the consumption of product inventory
</commit_message>
<xml_diff>
--- a/Resources/ZCustomaization.xlsx
+++ b/Resources/ZCustomaization.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="true" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -78,12 +78,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mmddyyyy"/>
     <numFmt numFmtId="165" formatCode="0_);\(0\)"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,12 +114,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="true" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -130,7 +130,7 @@
     <dxf>
       <font>
         <b/>
-        <i val="false"/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
@@ -140,8 +140,8 @@
     </dxf>
     <dxf>
       <font>
-        <b val="false"/>
-        <i val="false"/>
+        <b val="0"/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -151,11 +151,16 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="MySqlDefault" pivot="false" table="false" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -445,23 +450,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="15.28515625" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="15.28515625" bestFit="true" customWidth="true"/>
-    <col min="8" max="8" width="15.28515625" style="2" bestFit="true" customWidth="true"/>
-    <col min="9" max="9" width="9.7109375" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -478,7 +483,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -492,10 +497,10 @@
         <v>18</v>
       </c>
       <c r="E2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -506,7 +511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3013684357</v>
       </c>
@@ -522,7 +527,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3013695991</v>
       </c>
@@ -530,7 +535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>3013649705</v>
       </c>
@@ -538,7 +543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>3013410769</v>
       </c>
@@ -546,7 +551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>3013600797</v>
       </c>
@@ -554,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>3013650984</v>
       </c>
@@ -562,7 +567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>3013650989</v>
       </c>
@@ -570,7 +575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>3013667080</v>
       </c>
@@ -578,7 +583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>3013676007</v>
       </c>
@@ -586,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>3013696116</v>
       </c>
@@ -594,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>3013696125</v>
       </c>
@@ -602,7 +607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>3013696128</v>
       </c>
@@ -610,7 +615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>3013696132</v>
       </c>
@@ -618,7 +623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>3013696136</v>
       </c>
@@ -626,7 +631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>3013696159</v>
       </c>
@@ -634,7 +639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>3013410769</v>
       </c>
@@ -642,7 +647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>3013490006</v>
       </c>
@@ -650,7 +655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>3013527955</v>
       </c>
@@ -658,7 +663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>3013628150</v>
       </c>
@@ -666,7 +671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>3013629116</v>
       </c>
@@ -674,7 +679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>3013629139</v>
       </c>
@@ -689,27 +694,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -723,12 +728,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>